<commit_message>
push all data to DB
pushing all the data to DB with no visible bugs
</commit_message>
<xml_diff>
--- a/ex_sheets/oo.xlsx
+++ b/ex_sheets/oo.xlsx
@@ -12300,6 +12300,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12604,8 +12608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B467" workbookViewId="0">
-      <selection activeCell="D471" sqref="D471"/>
+    <sheetView tabSelected="1" topLeftCell="A2076" workbookViewId="0">
+      <selection activeCell="D2092" sqref="D2092"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>